<commit_message>
added interactive graphs and solver
</commit_message>
<xml_diff>
--- a/data/edgesNodes.xlsx
+++ b/data/edgesNodes.xlsx
@@ -40,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,12 +107,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,8 +139,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -153,7 +158,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -169,15 +174,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,12 +190,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>7</v>
@@ -198,91 +203,59 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>13</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>